<commit_message>
Added export to JSON
</commit_message>
<xml_diff>
--- a/docs/Finance/Finance model.xlsx
+++ b/docs/Finance/Finance model.xlsx
@@ -540,13 +540,13 @@
     <t>ExchangeRate_exchangeRateTypeId</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference (from) to currency </t>
+    <t>Reference (from) to currency</t>
   </si>
   <si>
     <t>ExchangeRate_fromCurrencyId</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference (to) to currency </t>
+    <t>Reference (to) to currency</t>
   </si>
   <si>
     <t>ExchangeRate_toCurrencyId</t>

</xml_diff>